<commit_message>
Sketching hinzugefügt, Projektmanagement aktualisiert
</commit_message>
<xml_diff>
--- a/03_Erarbeiten_von_Gestaltungsloesungen/Prototyping Verteilung.xlsx
+++ b/03_Erarbeiten_von_Gestaltungsloesungen/Prototyping Verteilung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carola\Desktop\OTH\HCI\HCI_OTH_APP\00_Projektmanagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\career\study\term6\human_computer_interactions\project_oth_app\03_Erarbeiten_von_Gestaltungsloesungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBC795A1-6841-4AEA-91C3-147D470657E7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE089D99-1A47-435C-9774-6750ED81E774}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12195" xr2:uid="{8883A8DC-43C1-48C8-A0AF-D64E7C9F4A05}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
   <si>
     <t>Prototyping Verteilung</t>
   </si>
@@ -106,13 +106,28 @@
   </si>
   <si>
     <t>Linda &amp; Caro</t>
+  </si>
+  <si>
+    <t>Sicht</t>
+  </si>
+  <si>
+    <t>Zuständig</t>
+  </si>
+  <si>
+    <t>Prototyping erledigt</t>
+  </si>
+  <si>
+    <t>Testszenario geschrieben</t>
+  </si>
+  <si>
+    <t>Nein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +165,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -202,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -248,21 +271,6 @@
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
@@ -324,6 +332,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -331,15 +389,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Eingabe" xfId="2" builtinId="20"/>
@@ -657,183 +721,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175C7942-AB5D-43FF-8745-E2B67D2A61D7}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>24</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>